<commit_message>
modify the run sub cases
</commit_message>
<xml_diff>
--- a/frontend/polls/templates/polls/Performance_Template.xlsx
+++ b/frontend/polls/templates/polls/Performance_Template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="705" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="705" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="algorithm" sheetId="1" r:id="rId1"/>
@@ -1333,10 +1333,6 @@
     <t>481.wrf</t>
   </si>
   <si>
-    <t>nbench</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>multicore_32_int</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
@@ -1362,6 +1358,10 @@
   </si>
   <si>
     <t>sec</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>spec</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -1583,6 +1583,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" indent="4"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1591,9 +1594,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" indent="4"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4108,13 +4108,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="A4:A9"/>
-    <mergeCell ref="B4:B9"/>
-    <mergeCell ref="C4:C9"/>
-    <mergeCell ref="A10:A17"/>
-    <mergeCell ref="B10:B17"/>
-    <mergeCell ref="C10:C17"/>
     <mergeCell ref="A50:A53"/>
     <mergeCell ref="B50:B53"/>
     <mergeCell ref="C50:C53"/>
@@ -4124,6 +4117,13 @@
     <mergeCell ref="C26:C33"/>
     <mergeCell ref="C34:C41"/>
     <mergeCell ref="C42:C49"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="B4:B9"/>
+    <mergeCell ref="C4:C9"/>
+    <mergeCell ref="A10:A17"/>
+    <mergeCell ref="B10:B17"/>
+    <mergeCell ref="C10:C17"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
@@ -4139,8 +4139,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMI90"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D71" sqref="D71:E71"/>
+    <sheetView showGridLines="0" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C72" sqref="C72:C90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38846,7 +38846,7 @@
         <v>11</v>
       </c>
       <c r="B58" s="24" t="s">
-        <v>436</v>
+        <v>443</v>
       </c>
       <c r="C58" s="24" t="s">
         <v>91</v>
@@ -39099,10 +39099,10 @@
       <c r="B71" s="25"/>
       <c r="C71" s="26"/>
       <c r="D71" s="6" t="s">
+        <v>441</v>
+      </c>
+      <c r="E71" s="6" t="s">
         <v>442</v>
-      </c>
-      <c r="E71" s="6" t="s">
-        <v>443</v>
       </c>
       <c r="F71" s="7"/>
       <c r="G71" s="7"/>
@@ -39466,10 +39466,10 @@
         <v>94</v>
       </c>
       <c r="D90" s="6" t="s">
+        <v>441</v>
+      </c>
+      <c r="E90" s="6" t="s">
         <v>442</v>
-      </c>
-      <c r="E90" s="6" t="s">
-        <v>443</v>
       </c>
       <c r="F90" s="7"/>
       <c r="G90" s="7"/>
@@ -39482,21 +39482,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="A6:A15"/>
-    <mergeCell ref="B6:B15"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="C9:C15"/>
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="B16:B18"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="A19:A31"/>
-    <mergeCell ref="B19:B31"/>
-    <mergeCell ref="C19:C22"/>
-    <mergeCell ref="C23:C27"/>
-    <mergeCell ref="C28:C31"/>
     <mergeCell ref="C72:C90"/>
     <mergeCell ref="A58:A90"/>
     <mergeCell ref="B58:B90"/>
@@ -39508,6 +39493,21 @@
     <mergeCell ref="C46:C51"/>
     <mergeCell ref="C52:C57"/>
     <mergeCell ref="C58:C71"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="A19:A31"/>
+    <mergeCell ref="B19:B31"/>
+    <mergeCell ref="C19:C22"/>
+    <mergeCell ref="C23:C27"/>
+    <mergeCell ref="C28:C31"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="A6:A15"/>
+    <mergeCell ref="B6:B15"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="C9:C15"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
@@ -39523,8 +39523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMI117"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B83" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="D65" sqref="D65:E65"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B28" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="C66" sqref="C66:C79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42999,7 +42999,7 @@
       <c r="A16" s="19">
         <v>4</v>
       </c>
-      <c r="B16" s="31" t="s">
+      <c r="B16" s="28" t="s">
         <v>149</v>
       </c>
       <c r="C16" s="20" t="s">
@@ -43024,7 +43024,7 @@
       <c r="A17" s="19">
         <v>10</v>
       </c>
-      <c r="B17" s="31" t="s">
+      <c r="B17" s="28" t="s">
         <v>149</v>
       </c>
       <c r="C17" s="20" t="s">
@@ -43049,7 +43049,7 @@
       <c r="A18" s="19">
         <v>10</v>
       </c>
-      <c r="B18" s="31" t="s">
+      <c r="B18" s="28" t="s">
         <v>149</v>
       </c>
       <c r="C18" s="20" t="s">
@@ -43074,7 +43074,7 @@
       <c r="A19" s="19">
         <v>10</v>
       </c>
-      <c r="B19" s="31" t="s">
+      <c r="B19" s="28" t="s">
         <v>149</v>
       </c>
       <c r="C19" s="20" t="s">
@@ -43099,7 +43099,7 @@
       <c r="A20" s="19">
         <v>10</v>
       </c>
-      <c r="B20" s="31" t="s">
+      <c r="B20" s="28" t="s">
         <v>149</v>
       </c>
       <c r="C20" s="20" t="s">
@@ -43124,7 +43124,7 @@
       <c r="A21" s="19">
         <v>10</v>
       </c>
-      <c r="B21" s="31" t="s">
+      <c r="B21" s="28" t="s">
         <v>149</v>
       </c>
       <c r="C21" s="20" t="s">
@@ -43149,7 +43149,7 @@
       <c r="A22" s="19">
         <v>10</v>
       </c>
-      <c r="B22" s="31" t="s">
+      <c r="B22" s="28" t="s">
         <v>149</v>
       </c>
       <c r="C22" s="20" t="s">
@@ -43174,7 +43174,7 @@
       <c r="A23" s="19">
         <v>10</v>
       </c>
-      <c r="B23" s="31" t="s">
+      <c r="B23" s="28" t="s">
         <v>149</v>
       </c>
       <c r="C23" s="20" t="s">
@@ -43199,7 +43199,7 @@
       <c r="A24" s="19">
         <v>10</v>
       </c>
-      <c r="B24" s="31" t="s">
+      <c r="B24" s="28" t="s">
         <v>149</v>
       </c>
       <c r="C24" s="20" t="s">
@@ -43224,7 +43224,7 @@
       <c r="A25" s="19">
         <v>10</v>
       </c>
-      <c r="B25" s="31" t="s">
+      <c r="B25" s="28" t="s">
         <v>149</v>
       </c>
       <c r="C25" s="20" t="s">
@@ -43249,7 +43249,7 @@
       <c r="A26" s="19">
         <v>10</v>
       </c>
-      <c r="B26" s="31" t="s">
+      <c r="B26" s="28" t="s">
         <v>149</v>
       </c>
       <c r="C26" s="20" t="s">
@@ -43274,7 +43274,7 @@
       <c r="A27" s="19">
         <v>10</v>
       </c>
-      <c r="B27" s="31" t="s">
+      <c r="B27" s="28" t="s">
         <v>149</v>
       </c>
       <c r="C27" s="20" t="s">
@@ -43299,7 +43299,7 @@
       <c r="A28" s="19">
         <v>10</v>
       </c>
-      <c r="B28" s="31" t="s">
+      <c r="B28" s="28" t="s">
         <v>149</v>
       </c>
       <c r="C28" s="20" t="s">
@@ -43324,7 +43324,7 @@
       <c r="A29" s="19">
         <v>10</v>
       </c>
-      <c r="B29" s="31" t="s">
+      <c r="B29" s="28" t="s">
         <v>149</v>
       </c>
       <c r="C29" s="20" t="s">
@@ -43349,7 +43349,7 @@
       <c r="A30" s="19">
         <v>10</v>
       </c>
-      <c r="B30" s="31" t="s">
+      <c r="B30" s="28" t="s">
         <v>149</v>
       </c>
       <c r="C30" s="20" t="s">
@@ -43374,7 +43374,7 @@
       <c r="A31" s="19">
         <v>10</v>
       </c>
-      <c r="B31" s="31" t="s">
+      <c r="B31" s="28" t="s">
         <v>149</v>
       </c>
       <c r="C31" s="20" t="s">
@@ -43399,7 +43399,7 @@
       <c r="A32" s="19">
         <v>10</v>
       </c>
-      <c r="B32" s="31" t="s">
+      <c r="B32" s="28" t="s">
         <v>149</v>
       </c>
       <c r="C32" s="20" t="s">
@@ -43424,7 +43424,7 @@
       <c r="A33" s="19">
         <v>10</v>
       </c>
-      <c r="B33" s="31" t="s">
+      <c r="B33" s="28" t="s">
         <v>149</v>
       </c>
       <c r="C33" s="20" t="s">
@@ -43449,7 +43449,7 @@
       <c r="A34" s="19">
         <v>10</v>
       </c>
-      <c r="B34" s="31" t="s">
+      <c r="B34" s="28" t="s">
         <v>149</v>
       </c>
       <c r="C34" s="20" t="s">
@@ -43474,7 +43474,7 @@
       <c r="A35" s="19">
         <v>10</v>
       </c>
-      <c r="B35" s="31" t="s">
+      <c r="B35" s="28" t="s">
         <v>149</v>
       </c>
       <c r="C35" s="20" t="s">
@@ -43499,7 +43499,7 @@
       <c r="A36" s="19">
         <v>10</v>
       </c>
-      <c r="B36" s="31" t="s">
+      <c r="B36" s="28" t="s">
         <v>149</v>
       </c>
       <c r="C36" s="20" t="s">
@@ -43524,7 +43524,7 @@
       <c r="A37" s="19">
         <v>10</v>
       </c>
-      <c r="B37" s="31" t="s">
+      <c r="B37" s="28" t="s">
         <v>149</v>
       </c>
       <c r="C37" s="20" t="s">
@@ -43549,7 +43549,7 @@
       <c r="A38" s="19">
         <v>10</v>
       </c>
-      <c r="B38" s="31" t="s">
+      <c r="B38" s="28" t="s">
         <v>149</v>
       </c>
       <c r="C38" s="20" t="s">
@@ -43574,7 +43574,7 @@
       <c r="A39" s="19">
         <v>10</v>
       </c>
-      <c r="B39" s="31" t="s">
+      <c r="B39" s="28" t="s">
         <v>149</v>
       </c>
       <c r="C39" s="20" t="s">
@@ -43599,7 +43599,7 @@
       <c r="A40" s="19">
         <v>10</v>
       </c>
-      <c r="B40" s="31" t="s">
+      <c r="B40" s="28" t="s">
         <v>149</v>
       </c>
       <c r="C40" s="20" t="s">
@@ -43624,7 +43624,7 @@
       <c r="A41" s="19">
         <v>10</v>
       </c>
-      <c r="B41" s="31" t="s">
+      <c r="B41" s="28" t="s">
         <v>149</v>
       </c>
       <c r="C41" s="20" t="s">
@@ -43649,7 +43649,7 @@
       <c r="A42" s="19">
         <v>10</v>
       </c>
-      <c r="B42" s="31" t="s">
+      <c r="B42" s="28" t="s">
         <v>149</v>
       </c>
       <c r="C42" s="20" t="s">
@@ -43674,7 +43674,7 @@
       <c r="A43" s="19">
         <v>10</v>
       </c>
-      <c r="B43" s="31" t="s">
+      <c r="B43" s="28" t="s">
         <v>149</v>
       </c>
       <c r="C43" s="20" t="s">
@@ -43699,7 +43699,7 @@
       <c r="A44" s="19">
         <v>10</v>
       </c>
-      <c r="B44" s="31" t="s">
+      <c r="B44" s="28" t="s">
         <v>149</v>
       </c>
       <c r="C44" s="20" t="s">
@@ -43724,7 +43724,7 @@
       <c r="A45" s="19">
         <v>10</v>
       </c>
-      <c r="B45" s="31" t="s">
+      <c r="B45" s="28" t="s">
         <v>149</v>
       </c>
       <c r="C45" s="20" t="s">
@@ -43749,7 +43749,7 @@
       <c r="A46" s="19">
         <v>10</v>
       </c>
-      <c r="B46" s="31" t="s">
+      <c r="B46" s="28" t="s">
         <v>149</v>
       </c>
       <c r="C46" s="20" t="s">
@@ -43774,7 +43774,7 @@
       <c r="A47" s="19">
         <v>10</v>
       </c>
-      <c r="B47" s="31" t="s">
+      <c r="B47" s="28" t="s">
         <v>149</v>
       </c>
       <c r="C47" s="20" t="s">
@@ -43799,7 +43799,7 @@
       <c r="A48" s="19">
         <v>10</v>
       </c>
-      <c r="B48" s="31" t="s">
+      <c r="B48" s="28" t="s">
         <v>149</v>
       </c>
       <c r="C48" s="20" t="s">
@@ -43824,7 +43824,7 @@
       <c r="A49" s="19">
         <v>10</v>
       </c>
-      <c r="B49" s="31" t="s">
+      <c r="B49" s="28" t="s">
         <v>149</v>
       </c>
       <c r="C49" s="20" t="s">
@@ -43849,7 +43849,7 @@
       <c r="A50" s="19">
         <v>10</v>
       </c>
-      <c r="B50" s="31" t="s">
+      <c r="B50" s="28" t="s">
         <v>149</v>
       </c>
       <c r="C50" s="20" t="s">
@@ -43874,7 +43874,7 @@
       <c r="A51" s="19">
         <v>10</v>
       </c>
-      <c r="B51" s="31" t="s">
+      <c r="B51" s="28" t="s">
         <v>149</v>
       </c>
       <c r="C51" s="20" t="s">
@@ -43896,11 +43896,11 @@
       <c r="M51" s="13"/>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B52" s="28" t="s">
+      <c r="B52" s="29" t="s">
+        <v>443</v>
+      </c>
+      <c r="C52" s="20" t="s">
         <v>436</v>
-      </c>
-      <c r="C52" s="20" t="s">
-        <v>437</v>
       </c>
       <c r="D52" s="6" t="s">
         <v>421</v>
@@ -43918,7 +43918,7 @@
       <c r="M52" s="7"/>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B53" s="29"/>
+      <c r="B53" s="30"/>
       <c r="C53" s="20" t="s">
         <v>91</v>
       </c>
@@ -43938,7 +43938,7 @@
       <c r="M53" s="7"/>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B54" s="29"/>
+      <c r="B54" s="30"/>
       <c r="C54" s="20" t="s">
         <v>91</v>
       </c>
@@ -43958,7 +43958,7 @@
       <c r="M54" s="7"/>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B55" s="29"/>
+      <c r="B55" s="30"/>
       <c r="C55" s="20"/>
       <c r="D55" s="6" t="s">
         <v>433</v>
@@ -43976,7 +43976,7 @@
       <c r="M55" s="7"/>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B56" s="29"/>
+      <c r="B56" s="30"/>
       <c r="C56" s="20" t="s">
         <v>91</v>
       </c>
@@ -43996,7 +43996,7 @@
       <c r="M56" s="7"/>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B57" s="29"/>
+      <c r="B57" s="30"/>
       <c r="C57" s="20"/>
       <c r="D57" s="6" t="s">
         <v>424</v>
@@ -44014,7 +44014,7 @@
       <c r="M57" s="7"/>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B58" s="29"/>
+      <c r="B58" s="30"/>
       <c r="C58" s="20"/>
       <c r="D58" s="6" t="s">
         <v>425</v>
@@ -44032,7 +44032,7 @@
       <c r="M58" s="7"/>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B59" s="29"/>
+      <c r="B59" s="30"/>
       <c r="C59" s="20"/>
       <c r="D59" s="6" t="s">
         <v>426</v>
@@ -44050,7 +44050,7 @@
       <c r="M59" s="7"/>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B60" s="29"/>
+      <c r="B60" s="30"/>
       <c r="C60" s="20"/>
       <c r="D60" s="6" t="s">
         <v>427</v>
@@ -44068,7 +44068,7 @@
       <c r="M60" s="7"/>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B61" s="29"/>
+      <c r="B61" s="30"/>
       <c r="C61" s="20"/>
       <c r="D61" s="6" t="s">
         <v>428</v>
@@ -44086,7 +44086,7 @@
       <c r="M61" s="7"/>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B62" s="29"/>
+      <c r="B62" s="30"/>
       <c r="C62" s="20" t="s">
         <v>91</v>
       </c>
@@ -44106,7 +44106,7 @@
       <c r="M62" s="7"/>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B63" s="29"/>
+      <c r="B63" s="30"/>
       <c r="C63" s="20" t="s">
         <v>91</v>
       </c>
@@ -44126,7 +44126,7 @@
       <c r="M63" s="7"/>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B64" s="29"/>
+      <c r="B64" s="30"/>
       <c r="C64" s="20"/>
       <c r="D64" s="6" t="s">
         <v>431</v>
@@ -44144,15 +44144,15 @@
       <c r="M64" s="7"/>
     </row>
     <row r="65" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B65" s="29"/>
+      <c r="B65" s="30"/>
       <c r="C65" s="20" t="s">
         <v>91</v>
       </c>
       <c r="D65" s="6" t="s">
+        <v>441</v>
+      </c>
+      <c r="E65" s="6" t="s">
         <v>442</v>
-      </c>
-      <c r="E65" s="6" t="s">
-        <v>443</v>
       </c>
       <c r="F65" s="7"/>
       <c r="G65" s="7"/>
@@ -44164,9 +44164,9 @@
       <c r="M65" s="7"/>
     </row>
     <row r="66" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B66" s="29"/>
+      <c r="B66" s="30"/>
       <c r="C66" s="24" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D66" s="6" t="s">
         <v>421</v>
@@ -44184,7 +44184,7 @@
       <c r="M66" s="7"/>
     </row>
     <row r="67" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B67" s="29"/>
+      <c r="B67" s="30"/>
       <c r="C67" s="25"/>
       <c r="D67" s="6" t="s">
         <v>422</v>
@@ -44202,7 +44202,7 @@
       <c r="M67" s="7"/>
     </row>
     <row r="68" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B68" s="29"/>
+      <c r="B68" s="30"/>
       <c r="C68" s="25"/>
       <c r="D68" s="6" t="s">
         <v>432</v>
@@ -44220,7 +44220,7 @@
       <c r="M68" s="7"/>
     </row>
     <row r="69" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B69" s="29"/>
+      <c r="B69" s="30"/>
       <c r="C69" s="25"/>
       <c r="D69" s="6" t="s">
         <v>433</v>
@@ -44238,7 +44238,7 @@
       <c r="M69" s="7"/>
     </row>
     <row r="70" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B70" s="29"/>
+      <c r="B70" s="30"/>
       <c r="C70" s="25"/>
       <c r="D70" s="6" t="s">
         <v>423</v>
@@ -44256,7 +44256,7 @@
       <c r="M70" s="7"/>
     </row>
     <row r="71" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B71" s="29"/>
+      <c r="B71" s="30"/>
       <c r="C71" s="25"/>
       <c r="D71" s="6" t="s">
         <v>424</v>
@@ -44274,7 +44274,7 @@
       <c r="M71" s="7"/>
     </row>
     <row r="72" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B72" s="29"/>
+      <c r="B72" s="30"/>
       <c r="C72" s="25"/>
       <c r="D72" s="6" t="s">
         <v>425</v>
@@ -44292,7 +44292,7 @@
       <c r="M72" s="7"/>
     </row>
     <row r="73" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B73" s="29"/>
+      <c r="B73" s="30"/>
       <c r="C73" s="25"/>
       <c r="D73" s="6" t="s">
         <v>426</v>
@@ -44310,7 +44310,7 @@
       <c r="M73" s="7"/>
     </row>
     <row r="74" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B74" s="29"/>
+      <c r="B74" s="30"/>
       <c r="C74" s="25"/>
       <c r="D74" s="6" t="s">
         <v>427</v>
@@ -44328,7 +44328,7 @@
       <c r="M74" s="7"/>
     </row>
     <row r="75" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B75" s="29"/>
+      <c r="B75" s="30"/>
       <c r="C75" s="25"/>
       <c r="D75" s="6" t="s">
         <v>428</v>
@@ -44346,7 +44346,7 @@
       <c r="M75" s="7"/>
     </row>
     <row r="76" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B76" s="29"/>
+      <c r="B76" s="30"/>
       <c r="C76" s="25"/>
       <c r="D76" s="6" t="s">
         <v>429</v>
@@ -44364,7 +44364,7 @@
       <c r="M76" s="7"/>
     </row>
     <row r="77" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B77" s="29"/>
+      <c r="B77" s="30"/>
       <c r="C77" s="25"/>
       <c r="D77" s="6" t="s">
         <v>430</v>
@@ -44382,7 +44382,7 @@
       <c r="M77" s="7"/>
     </row>
     <row r="78" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B78" s="29"/>
+      <c r="B78" s="30"/>
       <c r="C78" s="25"/>
       <c r="D78" s="6" t="s">
         <v>431</v>
@@ -44400,13 +44400,13 @@
       <c r="M78" s="7"/>
     </row>
     <row r="79" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B79" s="29"/>
+      <c r="B79" s="30"/>
       <c r="C79" s="25"/>
       <c r="D79" s="6" t="s">
+        <v>441</v>
+      </c>
+      <c r="E79" s="6" t="s">
         <v>442</v>
-      </c>
-      <c r="E79" s="6" t="s">
-        <v>443</v>
       </c>
       <c r="F79" s="7"/>
       <c r="G79" s="7"/>
@@ -44418,9 +44418,9 @@
       <c r="M79" s="7"/>
     </row>
     <row r="80" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B80" s="29"/>
+      <c r="B80" s="30"/>
       <c r="C80" s="20" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D80" s="6" t="s">
         <v>404</v>
@@ -44438,7 +44438,7 @@
       <c r="M80" s="7"/>
     </row>
     <row r="81" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B81" s="29"/>
+      <c r="B81" s="30"/>
       <c r="C81" s="20" t="s">
         <v>94</v>
       </c>
@@ -44458,7 +44458,7 @@
       <c r="M81" s="7"/>
     </row>
     <row r="82" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B82" s="29"/>
+      <c r="B82" s="30"/>
       <c r="C82" s="20"/>
       <c r="D82" s="6" t="s">
         <v>406</v>
@@ -44476,13 +44476,13 @@
       <c r="M82" s="7"/>
     </row>
     <row r="83" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B83" s="29"/>
+      <c r="B83" s="30"/>
       <c r="C83" s="20"/>
       <c r="D83" s="6" t="s">
         <v>407</v>
       </c>
       <c r="E83" s="6" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="F83" s="7"/>
       <c r="G83" s="7"/>
@@ -44494,7 +44494,7 @@
       <c r="M83" s="7"/>
     </row>
     <row r="84" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B84" s="29"/>
+      <c r="B84" s="30"/>
       <c r="C84" s="20"/>
       <c r="D84" s="6" t="s">
         <v>408</v>
@@ -44512,7 +44512,7 @@
       <c r="M84" s="7"/>
     </row>
     <row r="85" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B85" s="29"/>
+      <c r="B85" s="30"/>
       <c r="C85" s="20"/>
       <c r="D85" s="6" t="s">
         <v>409</v>
@@ -44530,7 +44530,7 @@
       <c r="M85" s="7"/>
     </row>
     <row r="86" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B86" s="29"/>
+      <c r="B86" s="30"/>
       <c r="C86" s="20"/>
       <c r="D86" s="6" t="s">
         <v>410</v>
@@ -44548,7 +44548,7 @@
       <c r="M86" s="7"/>
     </row>
     <row r="87" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B87" s="29"/>
+      <c r="B87" s="30"/>
       <c r="C87" s="20"/>
       <c r="D87" s="6" t="s">
         <v>411</v>
@@ -44566,7 +44566,7 @@
       <c r="M87" s="7"/>
     </row>
     <row r="88" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B88" s="29"/>
+      <c r="B88" s="30"/>
       <c r="C88" s="20"/>
       <c r="D88" s="6" t="s">
         <v>412</v>
@@ -44584,7 +44584,7 @@
       <c r="M88" s="7"/>
     </row>
     <row r="89" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B89" s="29"/>
+      <c r="B89" s="30"/>
       <c r="C89" s="20"/>
       <c r="D89" s="6" t="s">
         <v>413</v>
@@ -44602,7 +44602,7 @@
       <c r="M89" s="7"/>
     </row>
     <row r="90" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B90" s="29"/>
+      <c r="B90" s="30"/>
       <c r="C90" s="20"/>
       <c r="D90" s="6" t="s">
         <v>414</v>
@@ -44620,7 +44620,7 @@
       <c r="M90" s="7"/>
     </row>
     <row r="91" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B91" s="29"/>
+      <c r="B91" s="30"/>
       <c r="C91" s="20"/>
       <c r="D91" s="6" t="s">
         <v>415</v>
@@ -44638,7 +44638,7 @@
       <c r="M91" s="7"/>
     </row>
     <row r="92" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B92" s="29"/>
+      <c r="B92" s="30"/>
       <c r="C92" s="20"/>
       <c r="D92" s="6" t="s">
         <v>416</v>
@@ -44656,7 +44656,7 @@
       <c r="M92" s="7"/>
     </row>
     <row r="93" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B93" s="29"/>
+      <c r="B93" s="30"/>
       <c r="C93" s="20"/>
       <c r="D93" s="6" t="s">
         <v>417</v>
@@ -44674,7 +44674,7 @@
       <c r="M93" s="7"/>
     </row>
     <row r="94" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B94" s="29"/>
+      <c r="B94" s="30"/>
       <c r="C94" s="20"/>
       <c r="D94" s="6" t="s">
         <v>434</v>
@@ -44692,7 +44692,7 @@
       <c r="M94" s="7"/>
     </row>
     <row r="95" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B95" s="29"/>
+      <c r="B95" s="30"/>
       <c r="C95" s="20"/>
       <c r="D95" s="6" t="s">
         <v>435</v>
@@ -44710,7 +44710,7 @@
       <c r="M95" s="7"/>
     </row>
     <row r="96" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B96" s="29"/>
+      <c r="B96" s="30"/>
       <c r="C96" s="20"/>
       <c r="D96" s="6" t="s">
         <v>418</v>
@@ -44728,7 +44728,7 @@
       <c r="M96" s="7"/>
     </row>
     <row r="97" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B97" s="29"/>
+      <c r="B97" s="30"/>
       <c r="C97" s="20"/>
       <c r="D97" s="6" t="s">
         <v>419</v>
@@ -44746,15 +44746,15 @@
       <c r="M97" s="7"/>
     </row>
     <row r="98" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B98" s="29"/>
+      <c r="B98" s="30"/>
       <c r="C98" s="20" t="s">
         <v>94</v>
       </c>
       <c r="D98" s="6" t="s">
+        <v>441</v>
+      </c>
+      <c r="E98" s="6" t="s">
         <v>442</v>
-      </c>
-      <c r="E98" s="6" t="s">
-        <v>443</v>
       </c>
       <c r="F98" s="7"/>
       <c r="G98" s="7"/>
@@ -44766,9 +44766,9 @@
       <c r="M98" s="7"/>
     </row>
     <row r="99" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B99" s="29"/>
+      <c r="B99" s="30"/>
       <c r="C99" s="20" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D99" s="6" t="s">
         <v>404</v>
@@ -44786,7 +44786,7 @@
       <c r="M99" s="7"/>
     </row>
     <row r="100" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B100" s="29"/>
+      <c r="B100" s="30"/>
       <c r="C100" s="20"/>
       <c r="D100" s="6" t="s">
         <v>405</v>
@@ -44804,7 +44804,7 @@
       <c r="M100" s="7"/>
     </row>
     <row r="101" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B101" s="29"/>
+      <c r="B101" s="30"/>
       <c r="C101" s="20"/>
       <c r="D101" s="6" t="s">
         <v>406</v>
@@ -44822,13 +44822,13 @@
       <c r="M101" s="7"/>
     </row>
     <row r="102" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B102" s="29"/>
+      <c r="B102" s="30"/>
       <c r="C102" s="20"/>
       <c r="D102" s="6" t="s">
         <v>407</v>
       </c>
       <c r="E102" s="6" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="F102" s="7"/>
       <c r="G102" s="7"/>
@@ -44840,7 +44840,7 @@
       <c r="M102" s="7"/>
     </row>
     <row r="103" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B103" s="29"/>
+      <c r="B103" s="30"/>
       <c r="C103" s="20"/>
       <c r="D103" s="6" t="s">
         <v>408</v>
@@ -44858,7 +44858,7 @@
       <c r="M103" s="7"/>
     </row>
     <row r="104" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B104" s="29"/>
+      <c r="B104" s="30"/>
       <c r="C104" s="20"/>
       <c r="D104" s="6" t="s">
         <v>409</v>
@@ -44876,7 +44876,7 @@
       <c r="M104" s="7"/>
     </row>
     <row r="105" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B105" s="29"/>
+      <c r="B105" s="30"/>
       <c r="C105" s="20"/>
       <c r="D105" s="6" t="s">
         <v>410</v>
@@ -44894,7 +44894,7 @@
       <c r="M105" s="7"/>
     </row>
     <row r="106" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B106" s="29"/>
+      <c r="B106" s="30"/>
       <c r="C106" s="20"/>
       <c r="D106" s="6" t="s">
         <v>411</v>
@@ -44912,7 +44912,7 @@
       <c r="M106" s="7"/>
     </row>
     <row r="107" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B107" s="29"/>
+      <c r="B107" s="30"/>
       <c r="C107" s="20"/>
       <c r="D107" s="6" t="s">
         <v>412</v>
@@ -44930,7 +44930,7 @@
       <c r="M107" s="7"/>
     </row>
     <row r="108" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B108" s="29"/>
+      <c r="B108" s="30"/>
       <c r="C108" s="20"/>
       <c r="D108" s="6" t="s">
         <v>413</v>
@@ -44948,7 +44948,7 @@
       <c r="M108" s="7"/>
     </row>
     <row r="109" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B109" s="29"/>
+      <c r="B109" s="30"/>
       <c r="C109" s="20"/>
       <c r="D109" s="6" t="s">
         <v>414</v>
@@ -44966,7 +44966,7 @@
       <c r="M109" s="7"/>
     </row>
     <row r="110" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B110" s="29"/>
+      <c r="B110" s="30"/>
       <c r="C110" s="20"/>
       <c r="D110" s="6" t="s">
         <v>415</v>
@@ -44984,7 +44984,7 @@
       <c r="M110" s="7"/>
     </row>
     <row r="111" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B111" s="29"/>
+      <c r="B111" s="30"/>
       <c r="C111" s="20"/>
       <c r="D111" s="6" t="s">
         <v>416</v>
@@ -45002,7 +45002,7 @@
       <c r="M111" s="7"/>
     </row>
     <row r="112" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B112" s="29"/>
+      <c r="B112" s="30"/>
       <c r="C112" s="20"/>
       <c r="D112" s="6" t="s">
         <v>417</v>
@@ -45020,7 +45020,7 @@
       <c r="M112" s="7"/>
     </row>
     <row r="113" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B113" s="29"/>
+      <c r="B113" s="30"/>
       <c r="C113" s="20"/>
       <c r="D113" s="6" t="s">
         <v>434</v>
@@ -45038,7 +45038,7 @@
       <c r="M113" s="7"/>
     </row>
     <row r="114" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B114" s="29"/>
+      <c r="B114" s="30"/>
       <c r="C114" s="20"/>
       <c r="D114" s="6" t="s">
         <v>435</v>
@@ -45056,7 +45056,7 @@
       <c r="M114" s="7"/>
     </row>
     <row r="115" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B115" s="29"/>
+      <c r="B115" s="30"/>
       <c r="C115" s="20"/>
       <c r="D115" s="6" t="s">
         <v>418</v>
@@ -45074,7 +45074,7 @@
       <c r="M115" s="7"/>
     </row>
     <row r="116" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B116" s="29"/>
+      <c r="B116" s="30"/>
       <c r="C116" s="20"/>
       <c r="D116" s="6" t="s">
         <v>419</v>
@@ -45092,13 +45092,13 @@
       <c r="M116" s="7"/>
     </row>
     <row r="117" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B117" s="30"/>
+      <c r="B117" s="31"/>
       <c r="C117" s="20"/>
       <c r="D117" s="6" t="s">
+        <v>441</v>
+      </c>
+      <c r="E117" s="6" t="s">
         <v>442</v>
-      </c>
-      <c r="E117" s="6" t="s">
-        <v>443</v>
       </c>
       <c r="F117" s="7"/>
       <c r="G117" s="7"/>
@@ -45111,6 +45111,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="C52:C65"/>
+    <mergeCell ref="C80:C98"/>
+    <mergeCell ref="C66:C79"/>
+    <mergeCell ref="C99:C117"/>
+    <mergeCell ref="B52:B117"/>
     <mergeCell ref="A1:M1"/>
     <mergeCell ref="A4:A14"/>
     <mergeCell ref="B4:B14"/>
@@ -45122,11 +45127,6 @@
     <mergeCell ref="C34:C39"/>
     <mergeCell ref="C40:C45"/>
     <mergeCell ref="C46:C51"/>
-    <mergeCell ref="C52:C65"/>
-    <mergeCell ref="C80:C98"/>
-    <mergeCell ref="C66:C79"/>
-    <mergeCell ref="C99:C117"/>
-    <mergeCell ref="B52:B117"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
@@ -54493,19 +54493,6 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="A3:A16"/>
-    <mergeCell ref="B3:B16"/>
-    <mergeCell ref="C3:C6"/>
-    <mergeCell ref="C7:C16"/>
-    <mergeCell ref="C262:C290"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="A20:A36"/>
-    <mergeCell ref="B20:B45"/>
-    <mergeCell ref="C20:C36"/>
-    <mergeCell ref="C37:C45"/>
     <mergeCell ref="C291:C319"/>
     <mergeCell ref="B46:B319"/>
     <mergeCell ref="C46:C54"/>
@@ -54522,6 +54509,19 @@
     <mergeCell ref="C175:C203"/>
     <mergeCell ref="C204:C232"/>
     <mergeCell ref="C233:C261"/>
+    <mergeCell ref="C262:C290"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="A20:A36"/>
+    <mergeCell ref="B20:B45"/>
+    <mergeCell ref="C20:C36"/>
+    <mergeCell ref="C37:C45"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A3:A16"/>
+    <mergeCell ref="B3:B16"/>
+    <mergeCell ref="C3:C6"/>
+    <mergeCell ref="C7:C16"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
@@ -56179,18 +56179,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A26:A59"/>
+    <mergeCell ref="B26:B59"/>
+    <mergeCell ref="C26:C42"/>
+    <mergeCell ref="C43:C59"/>
+    <mergeCell ref="B60:B64"/>
+    <mergeCell ref="C60:C64"/>
     <mergeCell ref="A1:M1"/>
     <mergeCell ref="A3:A7"/>
     <mergeCell ref="B3:B7"/>
     <mergeCell ref="C3:C25"/>
     <mergeCell ref="A8:A25"/>
     <mergeCell ref="B8:B25"/>
-    <mergeCell ref="A26:A59"/>
-    <mergeCell ref="B26:B59"/>
-    <mergeCell ref="C26:C42"/>
-    <mergeCell ref="C43:C59"/>
-    <mergeCell ref="B60:B64"/>
-    <mergeCell ref="C60:C64"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>